<commit_message>
tests for the meat extravaganza pizza
</commit_message>
<xml_diff>
--- a/Pizza combinations, Adam Hale.xlsx
+++ b/Pizza combinations, Adam Hale.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25203"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="9220" yWindow="300" windowWidth="18140" windowHeight="11840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="7">
   <si>
     <t>Olives</t>
   </si>
@@ -35,17 +40,26 @@
   <si>
     <t>Y</t>
   </si>
+  <si>
+    <t>doesn’t put onions on it</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -69,9 +83,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -375,18 +392,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -436,7 +453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -489,7 +506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -542,7 +559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -595,7 +612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -611,7 +628,7 @@
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -620,36 +637,46 @@
       <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="K5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>5</v>
+      <c r="Q5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="F6" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -659,9 +686,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -671,8 +703,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>